<commit_message>
GUI and other fixes
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_2">Sheet1!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="114">
   <si>
     <t>Task</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Score</t>
-  </si>
-  <si>
-    <t>Stage, SpacmCounter</t>
   </si>
   <si>
     <t>ViewStageScanParams</t>
@@ -442,11 +439,50 @@
   <si>
     <t>DataCursor</t>
   </si>
+  <si>
+    <t>Stage, SpcmCounter</t>
+  </si>
+  <si>
+    <t>Needs more checks, but probably solved</t>
+  </si>
+  <si>
+    <t>Scan continousally without preparing and clearing spcm (check if needed)</t>
+  </si>
+  <si>
+    <t>Need to check what is the delay, if it is small, than no need</t>
+  </si>
+  <si>
+    <t>Move ToDo list to google drive</t>
+  </si>
+  <si>
+    <t>Reimplement Available Properties of ClassStage</t>
+  </si>
+  <si>
+    <t>ClassStage, StageAvailableProperties</t>
+  </si>
+  <si>
+    <t>I think it will simplify things. Maybe it is enough to have a "static property" for each stage</t>
+  </si>
+  <si>
+    <t>Not clear why this worked, but it seems legit</t>
+  </si>
+  <si>
+    <t>Fix SaveLoad</t>
+  </si>
+  <si>
+    <t>Needs to load struct to panel, after scan</t>
+  </si>
+  <si>
+    <t>Stage properties: hasCloseLoop, hasOpenLoop, hasJoystick</t>
+  </si>
+  <si>
+    <t>ClassStage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1120,14 +1156,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L42" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Accent6">
-  <autoFilter ref="A1:L42">
-    <filterColumn colId="10">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L47" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Accent6">
+  <autoFilter ref="A1:L47"/>
   <tableColumns count="12">
     <tableColumn id="11" name="#" dataDxfId="23" totalsRowDxfId="22"/>
     <tableColumn id="1" name="isDone" dataDxfId="21" totalsRowDxfId="20"/>
@@ -1411,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD42"/>
+  <dimension ref="A1:XFD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1436,16 +1466,16 @@
   <sheetData>
     <row r="1" spans="1:16384" s="2" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -1477,7 +1507,7 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23" t="str">
         <f ca="1">CONCATENATE("Open tasks: ",TEXT(COUNT(K:K),"#"))</f>
-        <v>Open tasks: 29</v>
+        <v>Open tasks: 30</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -1487,7 +1517,7 @@
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
@@ -17889,7 +17919,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="K3" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -17899,7 +17929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -17925,14 +17955,14 @@
         <v>9</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K4" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
@@ -17961,7 +17991,7 @@
         <v>9</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -17971,7 +18001,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -17997,7 +18027,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18018,7 +18048,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="5">
         <v>3</v>
@@ -18030,7 +18060,7 @@
         <v>9</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18063,10 +18093,10 @@
         <v>43009</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18081,7 +18111,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3">
         <v>3</v>
@@ -18096,20 +18126,20 @@
         <v>5</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="K9" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -18117,7 +18147,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="5">
         <v>8</v>
@@ -18135,14 +18165,14 @@
         <v>9</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:16384" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>9</v>
       </c>
@@ -18150,7 +18180,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="5">
         <v>10</v>
@@ -18168,7 +18198,7 @@
         <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18179,8 +18209,11 @@
       <c r="A12" s="13">
         <v>10</v>
       </c>
+      <c r="B12" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -18201,19 +18234,25 @@
         <v>9</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="6">
+        <v>32</v>
+      </c>
+      <c r="K12" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
-        <v>4</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:16384" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>11</v>
       </c>
+      <c r="B13" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -18234,11 +18273,11 @@
         <v>9</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="6">
+        <v>37</v>
+      </c>
+      <c r="K13" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
-        <v>2</v>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="14" spans="1:16384" ht="60.75" x14ac:dyDescent="0.3">
@@ -18246,7 +18285,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
@@ -18267,17 +18306,17 @@
         <v>9</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K14" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>0.5</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>13</v>
       </c>
@@ -18285,7 +18324,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
@@ -18303,17 +18342,17 @@
         <v>9</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K15" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>14</v>
       </c>
@@ -18321,7 +18360,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="5">
         <v>10</v>
@@ -18336,10 +18375,10 @@
         <v>43044</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K16" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18351,7 +18390,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3">
         <v>2</v>
@@ -18372,14 +18411,14 @@
         <v>9</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K17" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>0.5</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
@@ -18387,7 +18426,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -18408,14 +18447,14 @@
         <v>9</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K18" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -18423,7 +18462,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
@@ -18444,14 +18483,14 @@
         <v>9</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K19" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>18</v>
       </c>
@@ -18459,7 +18498,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -18477,7 +18516,7 @@
         <v>9</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18492,7 +18531,7 @@
         <v>0.5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="3">
         <v>2</v>
@@ -18513,7 +18552,7 @@
         <v>9</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K21" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18529,7 +18568,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5">
         <v>10</v>
@@ -18547,22 +18586,25 @@
         <v>9</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K22" s="6">
         <f ca="1">IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>5</v>
       </c>
       <c r="L22" s="15">
-        <v>43058</v>
+        <v>43062</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>21</v>
       </c>
+      <c r="B23" s="3">
+        <v>0.5</v>
+      </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3">
         <v>2</v>
@@ -18583,11 +18625,14 @@
         <v>9</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K23" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
-        <v>0.8</v>
+        <v>0.4</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -18595,7 +18640,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
@@ -18616,14 +18661,14 @@
         <v>9</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K24" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>1.5</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -18631,7 +18676,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="3">
         <v>2</v>
@@ -18652,7 +18697,7 @@
         <v>9</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K25" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18664,7 +18709,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="3">
         <v>2</v>
@@ -18685,14 +18730,14 @@
         <v>9</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K26" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>1.6</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -18700,7 +18745,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="3">
         <v>2</v>
@@ -18721,7 +18766,7 @@
         <v>9</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K27" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18733,7 +18778,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
@@ -18754,14 +18799,14 @@
         <v>9</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K28" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -18769,7 +18814,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -18790,17 +18835,17 @@
         <v>9</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K29" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>28</v>
       </c>
@@ -18808,7 +18853,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -18823,7 +18868,7 @@
         <v>9</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K30" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18834,8 +18879,11 @@
       <c r="A31" s="8">
         <v>29</v>
       </c>
+      <c r="B31" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="C31" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -18856,11 +18904,11 @@
         <v>9</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K31" s="6">
+        <v>76</v>
+      </c>
+      <c r="K31" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
-        <v>2.4</v>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -18868,7 +18916,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" s="3">
         <v>2</v>
@@ -18889,17 +18937,17 @@
         <v>9</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K32" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>0.5</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>31</v>
       </c>
@@ -18907,7 +18955,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" s="3">
         <v>2</v>
@@ -18928,7 +18976,7 @@
         <v>9</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K33" s="6" t="str">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -18942,7 +18990,7 @@
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="19">
         <v>1.5</v>
@@ -18960,7 +19008,7 @@
         <v>43055</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J34" s="19"/>
       <c r="K34" s="21">
@@ -18975,7 +19023,7 @@
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="19">
         <v>1.5</v>
@@ -18993,7 +19041,7 @@
         <v>43055</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J35" s="19"/>
       <c r="K35" s="21">
@@ -19007,7 +19055,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="3">
         <v>2</v>
@@ -19028,7 +19076,7 @@
         <v>9</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K36" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -19040,7 +19088,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D37" s="3">
         <v>2</v>
@@ -19061,14 +19109,14 @@
         <v>9</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K37" s="6">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>36</v>
       </c>
@@ -19076,7 +19124,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D38" s="22">
         <v>1</v>
@@ -19105,7 +19153,7 @@
       </c>
       <c r="B39" s="22"/>
       <c r="C39" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D39" s="22">
         <v>2</v>
@@ -19119,17 +19167,17 @@
         <v>43055</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J39" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K39" s="13">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>0</v>
       </c>
       <c r="L39" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -19138,7 +19186,7 @@
       </c>
       <c r="B40" s="19"/>
       <c r="C40" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40" s="19">
         <v>1.5</v>
@@ -19152,10 +19200,10 @@
         <v>43055</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K40" s="21">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
@@ -19169,7 +19217,7 @@
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="19">
         <v>2</v>
@@ -19187,17 +19235,17 @@
         <v>43058</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K41" s="21">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>1</v>
       </c>
       <c r="L41" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -19206,7 +19254,7 @@
       </c>
       <c r="B42" s="19"/>
       <c r="C42" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" s="19">
         <v>2</v>
@@ -19227,13 +19275,190 @@
         <v>9</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K42" s="21">
         <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
         <v>1</v>
       </c>
       <c r="L42" s="19"/>
+    </row>
+    <row r="43" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="18">
+        <v>40</v>
+      </c>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="19">
+        <v>2</v>
+      </c>
+      <c r="E43" s="18">
+        <v>2</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="18">
+        <v>5</v>
+      </c>
+      <c r="H43" s="20">
+        <v>43060</v>
+      </c>
+      <c r="I43" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K43" s="21">
+        <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L43" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
+        <v>41</v>
+      </c>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="E44" s="18">
+        <v>4</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="18">
+        <v>2</v>
+      </c>
+      <c r="H44" s="20">
+        <v>43060</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K44" s="21">
+        <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L44" s="19"/>
+    </row>
+    <row r="45" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="18">
+        <v>42</v>
+      </c>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="19">
+        <v>2</v>
+      </c>
+      <c r="E45" s="18">
+        <v>4</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="18">
+        <v>2</v>
+      </c>
+      <c r="H45" s="20">
+        <v>43062</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="K45" s="21">
+        <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L45" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="18">
+        <v>43</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="E46" s="18">
+        <v>5</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="18">
+        <v>3</v>
+      </c>
+      <c r="H46" s="20">
+        <v>43062</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K46" s="21">
+        <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
+        <v>2.5</v>
+      </c>
+      <c r="L46" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="18">
+        <v>44</v>
+      </c>
+      <c r="B47" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="19"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="18"/>
+      <c r="H47" s="20">
+        <v>43062</v>
+      </c>
+      <c r="I47" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="K47" s="21" t="str">
+        <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="L47" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K1048576 K1">

</xml_diff>

<commit_message>
Nadav's pedantic about grammar
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_2">Sheet1!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="119">
   <si>
     <t>Task</t>
   </si>
@@ -478,11 +478,26 @@
   <si>
     <t>ClassStage</t>
   </si>
+  <si>
+    <t>Get good colormaps for GUI</t>
+  </si>
+  <si>
+    <t>ViewImageResultPanelColormap</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/matlab/comments/1jqk8t/you_should_never_use_the_default_colors_in_matlab/</t>
+  </si>
+  <si>
+    <t>Implement lasers for setup 4</t>
+  </si>
+  <si>
+    <t>Laser?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,7 +607,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -664,6 +679,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1156,8 +1177,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L47" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Accent6">
-  <autoFilter ref="A1:L47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L49" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Accent6">
+  <autoFilter ref="A1:L49">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1.5"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="11" name="#" dataDxfId="23" totalsRowDxfId="22"/>
     <tableColumn id="1" name="isDone" dataDxfId="21" totalsRowDxfId="20"/>
@@ -1441,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD47"/>
+  <dimension ref="A1:XFD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1502,12 +1534,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" s="24" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23" t="str">
         <f ca="1">CONCATENATE("Open tasks: ",TEXT(COUNT(K:K),"#"))</f>
-        <v>Open tasks: 30</v>
+        <v>Open tasks: 32</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -17893,7 +17925,7 @@
       <c r="XFC2" s="23"/>
       <c r="XFD2" s="23"/>
     </row>
-    <row r="3" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -17929,7 +17961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -17965,7 +17997,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -18001,7 +18033,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -18034,7 +18066,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:16384" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16384" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -18070,7 +18102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -18106,7 +18138,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -18139,7 +18171,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -18172,7 +18204,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>9</v>
       </c>
@@ -18205,7 +18237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>10</v>
       </c>
@@ -18244,7 +18276,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16384" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>11</v>
       </c>
@@ -18280,7 +18312,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:16384" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16384" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>12</v>
       </c>
@@ -18316,7 +18348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:16384" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16384" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>13</v>
       </c>
@@ -18352,7 +18384,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16384" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>14</v>
       </c>
@@ -18385,7 +18417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>15</v>
       </c>
@@ -18421,7 +18453,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>16</v>
       </c>
@@ -18457,7 +18489,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>17</v>
       </c>
@@ -18490,7 +18522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>18</v>
       </c>
@@ -18523,7 +18555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>19</v>
       </c>
@@ -18559,7 +18591,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>20</v>
       </c>
@@ -18596,7 +18628,7 @@
         <v>43062</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>21</v>
       </c>
@@ -18635,7 +18667,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>22</v>
       </c>
@@ -18671,7 +18703,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -18704,7 +18736,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -18740,7 +18772,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -18773,7 +18805,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -18806,7 +18838,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -18845,7 +18877,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>28</v>
       </c>
@@ -18875,7 +18907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>29</v>
       </c>
@@ -18911,7 +18943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -18947,7 +18979,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>31</v>
       </c>
@@ -19050,7 +19082,7 @@
       </c>
       <c r="L35" s="19"/>
     </row>
-    <row r="36" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>34</v>
       </c>
@@ -19083,7 +19115,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>35</v>
       </c>
@@ -19116,7 +19148,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>36</v>
       </c>
@@ -19147,7 +19179,7 @@
       </c>
       <c r="L38" s="22"/>
     </row>
-    <row r="39" spans="1:12" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>37</v>
       </c>
@@ -19211,7 +19243,7 @@
       </c>
       <c r="L40" s="19"/>
     </row>
-    <row r="41" spans="1:12" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="121.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18">
         <v>39</v>
       </c>
@@ -19248,7 +19280,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
         <v>39</v>
       </c>
@@ -19283,7 +19315,7 @@
       </c>
       <c r="L42" s="19"/>
     </row>
-    <row r="43" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
         <v>40</v>
       </c>
@@ -19355,7 +19387,7 @@
       </c>
       <c r="L44" s="19"/>
     </row>
-    <row r="45" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18">
         <v>42</v>
       </c>
@@ -19429,7 +19461,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="40.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
         <v>44</v>
       </c>
@@ -19459,6 +19491,78 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="L47" s="19"/>
+    </row>
+    <row r="48" spans="1:12" ht="60.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18">
+        <v>45</v>
+      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="19">
+        <v>2</v>
+      </c>
+      <c r="E48" s="18">
+        <v>3</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="H48" s="20">
+        <v>43066</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="K48" s="21">
+        <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
+        <v>1.2</v>
+      </c>
+      <c r="L48" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="18">
+        <v>45</v>
+      </c>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="E49" s="18">
+        <v>5</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="18">
+        <v>2</v>
+      </c>
+      <c r="H49" s="20">
+        <v>43066</v>
+      </c>
+      <c r="I49" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="K49" s="21">
+        <f>IF(OR(ISBLANK(Table2[[#This Row],[Task]]),Table2[[#This Row],[isDone]]=TRUE)," ",Table2[[#This Row],[Priority]]*(1+COUNTIF(Table2[[#This Row],[Bug / Feature]],"Bug"))*(1-Table2[[#This Row],[isDone]])/(1+Table2[[#This Row],[Difficulty]]))</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L49" s="27"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K1048576 K1">
@@ -19473,11 +19577,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="L48" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>